<commit_message>
working on final figures
</commit_message>
<xml_diff>
--- a/results/tables/table_S5.xlsx
+++ b/results/tables/table_S5.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="332">
   <si>
     <t xml:space="preserve">Background</t>
   </si>
@@ -608,7 +608,13 @@
     <t xml:space="preserve">Substrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Median flux</t>
+    <t xml:space="preserve">Median optimal flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00276_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Glucosamine</t>
   </si>
   <si>
     <t xml:space="preserve">EX_cpd00001_e</t>
@@ -617,64 +623,322 @@
     <t xml:space="preserve">H2O</t>
   </si>
   <si>
+    <t xml:space="preserve">EX_cpd00023_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Glutamate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00971_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00051_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Arginine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd10515_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe2+</t>
+  </si>
+  <si>
     <t xml:space="preserve">EX_cpd00009_e</t>
   </si>
   <si>
     <t xml:space="preserve">Phosphate</t>
   </si>
   <si>
+    <t xml:space="preserve">EX_cpd00076_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sucrose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00067_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00122_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Acetyl-D-glucosamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00035_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Alanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00220_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riboflavin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00117_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Alanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00307_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00254_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00205_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00305_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00065_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Tryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00149_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00099_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00104_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biotin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00162_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aminoethanol</t>
+  </si>
+  <si>
     <t xml:space="preserve">EX_cpd00011_e</t>
   </si>
   <si>
     <t xml:space="preserve">CO2</t>
   </si>
   <si>
+    <t xml:space="preserve">EX_cpd00063_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd01080_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Octadecanoic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00156_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Valine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00039_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Lysine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00393_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00322_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Isoleucine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00030_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mn2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00516_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meso-2,6-Diaminopimelate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00644_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantothenate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00263_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyridoxol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00232_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Acetyl-Neuraminic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00107_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Leucine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00066_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Phenylalanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00492_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Acetyl-D-mannosamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00567_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Proline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00132_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Asparagine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00054_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Serine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00161_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Threonine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00041_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Aspartate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd19585_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Methylbutyrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00339_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-Aminopentanoate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd03170_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Hydroxymandelate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00036_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Succinate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00029_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00141_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propionate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00133_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicotinamide</t>
+  </si>
+  <si>
     <t xml:space="preserve">EX_cpd00013_e</t>
   </si>
   <si>
     <t xml:space="preserve">Ammonia</t>
   </si>
   <si>
-    <t xml:space="preserve">EX_cpd00023_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Glutamate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00029_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acetate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00030_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mn2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00035_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Alanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00036_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Succinate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00039_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Lysine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00041_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Aspartate</t>
+    <t xml:space="preserve">EX_cpd00443_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Aminobenzoate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd02711_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-keto-3-deoxygluconate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00072_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-fructose-6-phosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00136_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Hydroxybenzoate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd03561_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Hydroxybutyrate</t>
   </si>
   <si>
     <t xml:space="preserve">EX_cpd00047_e</t>
@@ -683,76 +947,10 @@
     <t xml:space="preserve">Formate</t>
   </si>
   <si>
-    <t xml:space="preserve">EX_cpd00051_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Arginine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00054_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Serine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00060_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Methionine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00063_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ca2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00065_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Tryptophan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00066_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Phenylalanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00067_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00072_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-fructose-6-phosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00076_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sucrose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00084_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Cysteine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00099_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cl-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00104_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biotin</t>
+    <t xml:space="preserve">EX_cpd00311_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guanosine</t>
   </si>
   <si>
     <t xml:space="preserve">EX_cpd00106_e</t>
@@ -761,76 +959,28 @@
     <t xml:space="preserve">Fumarate</t>
   </si>
   <si>
-    <t xml:space="preserve">EX_cpd00107_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Leucine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00117_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Alanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00119_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Histidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00122_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-Acetyl-D-glucosamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00132_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Asparagine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00133_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotinamide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00136_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-Hydroxybenzoate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00141_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propionate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00139_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycolate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00149_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00156_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Valine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00161_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Threonine</t>
+    <t xml:space="preserve">EX_cpd00277_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxyguanosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00654_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxycytidine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00412_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxyuridine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00438_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxyadenosine</t>
   </si>
   <si>
     <t xml:space="preserve">EX_cpd00182_e</t>
@@ -845,190 +995,28 @@
     <t xml:space="preserve">D-Glutamate</t>
   </si>
   <si>
-    <t xml:space="preserve">EX_cpd00162_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aminoethanol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00205_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K+</t>
-  </si>
-  <si>
     <t xml:space="preserve">EX_cpd00207_e</t>
   </si>
   <si>
     <t xml:space="preserve">Guanine</t>
   </si>
   <si>
-    <t xml:space="preserve">EX_cpd00220_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riboflavin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00232_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-Acetyl-Neuraminic acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00254_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00263_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyridoxol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00276_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Glucosamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00277_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyguanosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00305_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00307_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00311_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guanosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00320_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Aspartate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00322_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Isoleucine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00393_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00412_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyuridine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00424_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cystathionine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00443_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-Aminobenzoate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00438_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyadenosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00516_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meso-2,6-Diaminopimelate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00567_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Proline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00644_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantothenate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00654_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxycytidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd00971_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd01080_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Octadecanoic acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd02711_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-keto-3-deoxygluconate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd03170_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-Hydroxymandelate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd03561_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-Hydroxybutyrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd10515_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fe2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EX_cpd19585_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-Methylbutyrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK_cpd11416_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass</t>
+    <t xml:space="preserve">EX_cpd11584_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ala-His</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd01017_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cys-Gly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd11591_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gly-Met</t>
   </si>
 </sst>
 </file>
@@ -1132,7 +1120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1159,10 +1147,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -4800,19 +4784,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4824,22 +4810,22 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4851,7 +4837,7 @@
         <v>197</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>724.529504956759</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>196</v>
@@ -4860,7 +4846,7 @@
         <v>197</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>762.567255660645</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4871,7 +4857,7 @@
         <v>199</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>771.655927628327</v>
+        <v>477.778506253787</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>198</v>
@@ -4880,7 +4866,7 @@
         <v>199</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>966.916831973798</v>
+        <v>683.357495355627</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4891,7 +4877,7 @@
         <v>201</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>858.369069822663</v>
+        <v>-15.6233341884122</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>200</v>
@@ -4900,7 +4886,7 @@
         <v>201</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>964.140405420952</v>
+        <v>-15.8454458139179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4911,7 +4897,7 @@
         <v>203</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0</v>
+        <v>-0.0802019208855849</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>202</v>
@@ -4920,7 +4906,7 @@
         <v>203</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>510.60905100784</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,16 +4917,16 @@
         <v>205</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>-19.4955433726516</v>
+        <v>-5.1329229366446</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1000</v>
+        <v>-5.20589595529134</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4951,16 +4937,16 @@
         <v>207</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1000</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>-0.0813421243013863</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4971,16 +4957,16 @@
         <v>209</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>394.148020891348</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>-67.7478097394866</v>
+        <v>749.234053702535</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4991,16 +4977,16 @@
         <v>211</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>-70.6163008405674</v>
+        <v>-0.120302881327461</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>-370.624231593846</v>
+        <v>-0.122013186452023</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5011,16 +4997,16 @@
         <v>213</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>-33.7606078873707</v>
+        <v>-526.920174229948</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>-46.3557859158499</v>
+        <v>-983.378417645807</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,16 +5017,16 @@
         <v>215</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>-48.3185233075765</v>
+        <v>745.555169010648</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>-876.839942254272</v>
+        <v>999.999999999981</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5051,16 +5037,16 @@
         <v>217</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>-932.845611320258</v>
+        <v>-54.4089831284315</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>999.999999999998</v>
+        <v>-55.1824971260869</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5071,16 +5057,16 @@
         <v>219</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>1000</v>
+        <v>-0.0882221129736536</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>-6.14492605346823</v>
+        <v>-0.0894763367315363</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,16 +5077,16 @@
         <v>221</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>-6.40510665220575</v>
+        <v>-84.2120169293238</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>-354.675840109379</v>
+        <v>-85.4092305164967</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5111,147 +5097,147 @@
         <v>223</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>-460.294551929487</v>
+        <v>273.528651178531</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>-5.18478135761359</v>
+        <v>111.015370636713</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>-0.0802019208849742</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>-1.28102133044115</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>-1.22898521069374</v>
+        <v>-0.0813421243013863</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>-8.76698973020643</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>-8.41086753568436</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>-985.06705587541</v>
+        <v>-1.02658458732901</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>-933.293625526711</v>
+        <v>-1.04117919105829</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>-241.955844404578</v>
+        <v>-0.0802019208849742</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>-329.239294518933</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>-0.150119687161123</v>
+        <v>-0.0802019208849742</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>-0.144021704378019</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>-2.59206659831477</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>238</v>
@@ -5260,7 +5246,7 @@
         <v>239</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>-2.48677476226351</v>
+        <v>-227.085921605548</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5271,16 +5257,16 @@
         <v>241</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>633.043827332322</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>-0.0813421243013863</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5291,16 +5277,16 @@
         <v>243</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>-0.100079791440862</v>
+        <v>-0.0802019208849742</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>-0.0960144695854979</v>
+        <v>593.489249650051</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5311,16 +5297,16 @@
         <v>245</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>2.16427846855658E-012</v>
+        <v>-0.040100960442535</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>288.14962493677</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5331,16 +5317,16 @@
         <v>247</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>-18.2145220422099</v>
+        <v>-10.5224920201213</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>-17.4746334645498</v>
+        <v>-0.0406710621509774</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5351,16 +5337,16 @@
         <v>249</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>-105.083781012749</v>
+        <v>-38.7214874033117</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>-100.815193064711</v>
+        <v>-10.672086708347</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5371,16 +5357,16 @@
         <v>251</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>-2.72217032718731</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>-2.6115935727239</v>
+        <v>-39.2719776127281</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5391,16 +5377,16 @@
         <v>253</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>539.188028143765</v>
+        <v>-660.364631097423</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>825.477249393629</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5411,16 +5397,16 @@
         <v>255</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>-12.8902771375638</v>
+        <v>-0.0802019208849742</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>-12.3666636826044</v>
+        <v>-723.35398412688</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5431,16 +5417,16 @@
         <v>257</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>-0.500398957203856</v>
+        <v>-24.060576265521</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>-0.480072347928058</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5451,16 +5437,16 @@
         <v>259</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>-194.329828782082</v>
+        <v>-0.168424033859083</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>-151.384750373813</v>
+        <v>-24.4026372904276</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5471,27 +5457,27 @@
         <v>261</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>794.054429475137</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>0</v>
+        <v>-0.170818461033491</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>-48.9231717398928</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>260</v>
@@ -5500,47 +5486,47 @@
         <v>261</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>500.028590508358</v>
+        <v>-0.0813421243013863</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>-13.1304686370216</v>
+        <v>-14.5967496010827</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>-341.705878655579</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>-7.02568826953211</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="F37" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="C37" s="0" t="n">
-        <v>-9.92791531091871</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>267</v>
-      </c>
       <c r="G37" s="0" t="n">
-        <v>-12.5970984096095</v>
+        <v>-9.26547727431171E-012</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5551,16 +5537,16 @@
         <v>271</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>12.0780715837495</v>
+        <v>-170.022622405604</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>-9.52463538287554</v>
+        <v>-14.8042666228595</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5571,27 +5557,27 @@
         <v>273</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>-60.0478748644281</v>
+        <v>-10.3300074099969</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>-96.0995894018512</v>
+        <v>-7.12557008880481</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>-0.100079791440862</v>
+        <v>-447.327172863492</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>270</v>
@@ -5600,18 +5586,18 @@
         <v>271</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>-6.502841112032</v>
+        <v>-4.45754841171811</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>402.641619116222</v>
+        <v>-7.9560305517989</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>272</v>
@@ -5620,98 +5606,98 @@
         <v>273</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>-57.6086817512632</v>
+        <v>-10.4768656100237</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>-0.110087770584983</v>
+        <v>-9.17509974925213</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>-0.0960144695854979</v>
+        <v>-471.128845528021</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>-61.0486727788351</v>
+        <v>643.251123779831</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>-0.105615916544025</v>
+        <v>-8.06913873070141</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>165.626167579595</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>-391.911171154698</v>
+        <v>137.826058815452</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>-0.100079791440862</v>
+        <v>135.117117540155</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>707.135686243187</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>22.3478689884374</v>
+        <v>-1.56393745726029</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>286</v>
@@ -5720,18 +5706,18 @@
         <v>287</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>-0.0960144695854979</v>
+        <v>-374.571563438664</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>-385.219008984908</v>
+        <v>717.388343538471</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>288</v>
@@ -5740,18 +5726,18 @@
         <v>289</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>941.099765854908</v>
       </c>
       <c r="E48" s="0" t="s">
         <v>290</v>
@@ -5760,27 +5746,27 @@
         <v>291</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>-1.47862283161578</v>
+        <v>753.580301296008</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>-0.401009604425781</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="C49" s="0" t="n">
-        <v>341.322128708552</v>
-      </c>
-      <c r="E49" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>293</v>
-      </c>
       <c r="G49" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>708.199572071669</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5791,16 +5777,16 @@
         <v>297</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>-22.5873243823969</v>
+        <v>-0.0802019208852016</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>162.5414169717</v>
+        <v>-0.406710621508182</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5811,7 +5797,7 @@
         <v>299</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>999.99999999996</v>
+        <v>-276.135213607297</v>
       </c>
       <c r="E51" s="0" t="s">
         <v>296</v>
@@ -5820,7 +5806,7 @@
         <v>297</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>-3.57951736090411</v>
+        <v>-0.0813421243015</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5831,7 +5817,7 @@
         <v>301</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>-721.934033735707</v>
+        <v>-159.71019824412</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>298</v>
@@ -5840,7 +5826,7 @@
         <v>299</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>999.999999999999</v>
+        <v>-403.317078572596</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5851,7 +5837,7 @@
         <v>303</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>-142.162417818046</v>
       </c>
       <c r="E53" s="0" t="s">
         <v>300</v>
@@ -5860,7 +5846,7 @@
         <v>301</v>
       </c>
       <c r="G53" s="0" t="n">
-        <v>-725.125234721618</v>
+        <v>-389.771163700842</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5871,7 +5857,7 @@
         <v>305</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>-359.778057218887</v>
+        <v>-939.488090447366</v>
       </c>
       <c r="E54" s="0" t="s">
         <v>302</v>
@@ -5880,7 +5866,7 @@
         <v>303</v>
       </c>
       <c r="G54" s="0" t="n">
-        <v>-0.0960144695853842</v>
+        <v>-6.76766474187855</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5891,7 +5877,7 @@
         <v>307</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>-5.40430873779837</v>
+        <v>971.110225704748</v>
       </c>
       <c r="E55" s="0" t="s">
         <v>304</v>
@@ -5900,7 +5886,7 @@
         <v>305</v>
       </c>
       <c r="G55" s="0" t="n">
-        <v>-180.627485008525</v>
+        <v>-612.961070164531</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5911,7 +5897,7 @@
         <v>309</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>-0.100079791440749</v>
+        <v>-278.177860918798</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>310</v>
@@ -5920,7 +5906,7 @@
         <v>311</v>
       </c>
       <c r="G56" s="0" t="n">
-        <v>18.0902916855589</v>
+        <v>203.474424211537</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5931,16 +5917,16 @@
         <v>313</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>-30.0239374322141</v>
+        <v>-404.012563331317</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>-0.0960144695853842</v>
+        <v>999.999999999998</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5951,16 +5937,16 @@
         <v>315</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>-5.48437257095111</v>
+        <v>-2.52636050787953</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="G58" s="0" t="n">
-        <v>-28.8043408756317</v>
+        <v>-3.03251736292395</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5971,16 +5957,16 @@
         <v>317</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>-0.210167562025731</v>
+        <v>-288.318859041059</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G59" s="0" t="n">
-        <v>-23.9652116085259</v>
+        <v>-1.25266871424196</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5991,107 +5977,107 @@
         <v>319</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>-3.15251343038244</v>
+        <v>9.67912230490401</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="G60" s="0" t="n">
-        <v>-0.201630386130205</v>
+        <v>-5.50911661890029</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>-0.100079791440635</v>
+        <v>-48.1211525310418</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="G61" s="0" t="n">
-        <v>-3.02445579194114</v>
+        <v>-2.56227691549486</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>-0.0500398957203743</v>
+        <v>698.134941166247</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="G62" s="0" t="n">
-        <v>-0.0960144695856116</v>
+        <v>-126.896945765432</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>-565.541586204798</v>
+        <v>-2.18149224807382</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G63" s="0" t="n">
-        <v>-0.0480072347927489</v>
+        <v>15.3258437117798</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>185.734202038113</v>
+        <v>-2.07722975092349</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G64" s="0" t="n">
-        <v>-634.97256248507</v>
+        <v>-48.8052745808552</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>-729.739982142285</v>
+        <v>-4.33090372779373</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>326</v>
@@ -6100,19 +6086,10 @@
         <v>327</v>
       </c>
       <c r="G65" s="0" t="n">
-        <v>143.396346504304</v>
+        <v>-2.21250578099875</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="C66" s="0" t="n">
-        <v>-0.100079791440862</v>
-      </c>
       <c r="E66" s="0" t="s">
         <v>328</v>
       </c>
@@ -6120,19 +6097,10 @@
         <v>329</v>
       </c>
       <c r="G66" s="0" t="n">
-        <v>-426.092147857196</v>
+        <v>-2.10676101940749</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="C67" s="0" t="n">
-        <v>700.8058355168</v>
-      </c>
       <c r="E67" s="0" t="s">
         <v>330</v>
       </c>
@@ -6140,41 +6108,34 @@
         <v>331</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>-0.0960144695854979</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="C68" s="0" t="n">
-        <v>100.079791440713</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="G68" s="0" t="n">
-        <v>705.999152380198</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E69" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="G69" s="0" t="n">
-        <v>96.0144695854385</v>
+        <v>-4.39247471227702</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:C65">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G67">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00A933"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
updates for next submission
</commit_message>
<xml_diff>
--- a/results/tables/table_S5.xlsx
+++ b/results/tables/table_S5.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="context-specific essential gene" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="exchange fluxes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="RIPTiDe parameters" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="exchange fluxes - high spore" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="exchange fluxes - low spore" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="RIPTiDe parameters" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="360">
   <si>
     <t xml:space="preserve">Background</t>
   </si>
@@ -45,6 +46,150 @@
     <t xml:space="preserve">ABC transporter, substrate-binding protein (cluster 3, basic aa/glutamine/opines)</t>
   </si>
   <si>
+    <t xml:space="preserve">272563.8.peg.2720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyrimidine operon regulatory protein PyrR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP synthase gamma chain (EC 3.6.3.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glucose-6-phosphate isomerase (EC 5.3.1.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methionyl-tRNA synthetase (EC 6.1.1.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS system, glucitol/sorbitol-specific IIB component (EC 2.7.1.198) / PTS system, glucitol/sorbitol-specific IIC component 2 | srlE_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glycine reductase component B beta subunit (EC 1.21.4.2) / Glycine reductase component B alpha subunit (EC 1.21.4.2) | grdE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manganese-dependent inorganic pyrophosphatase (EC 3.6.1.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate-specific component TrpP of tryptophan ECF transporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purine nucleoside phosphorylase (EC 2.4.2.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP synthase beta chain (EC 3.6.3.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triosephosphate isomerase (EC 5.3.1.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valyl-tRNA synthetase (EC 6.1.1.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.866</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutamate synthase [NADPH] large chain (EC 1.4.1.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glycine cleavage system H protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1382</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riboflavin kinase (EC 2.7.1.26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2754</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glycerol-3-phosphate dehydrogenase [NAD(P)+] (EC 1.1.1.94)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP synthase alpha chain (EC 3.6.3.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isoleucyl-tRNA synthetase (EC 6.1.1.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cytidine deaminase (EC 3.5.4.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1061</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetylgalactosamine-6-phosphate deacetylase | nagA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphoribosylamine--glycine ligase (EC 6.3.4.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphoenolpyruvate-protein phosphotransferase of PTS system (EC 2.7.3.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alanine transaminase (EC 2.6.1.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leucyl-tRNA synthetase (EC 6.1.1.4)</t>
+  </si>
+  <si>
     <t xml:space="preserve">272563.8.peg.1085</t>
   </si>
   <si>
@@ -57,16 +202,112 @@
     <t xml:space="preserve">methylenetetrahydrofolate dehydrogenase (NADP+) (EC 1.5.1.5)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-hydroxybutyrate:acetyl-CoA CoA transferase (EC 2.3.1.-)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3708</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Methionyl-tRNA synthetase (EC 6.1.1.10)</t>
+    <t xml:space="preserve">272563.8.peg.3565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDP-N-acetylenolpyruvoylglucosamine reductase (EC 1.1.1.158)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aspartate carbamoyltransferase (EC 2.1.3.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP synthase epsilon chain (EC 3.6.3.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphoribosylformylglycinamidine synthase, glutamine amidotransferase subunit (EC 6.3.5.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sodium-solute symporter, putative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP synthase delta chain (EC 3.6.3.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDP-N-acetylmuramoylalanine--D-glutamate ligase (EC 6.3.2.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trehalose-6-phosphate hydrolase (EC 3.2.1.93)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetylneuraminate lyase (EC 4.1.3.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-deoxy-D-xylulose 5-phosphate synthase (EC 2.2.1.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adenine phosphoribosyltransferase (EC 2.4.2.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-aspartate oxidase (EC 1.4.3.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CDP-diacylglycerol--glycerol-3-phosphate 3-phosphatidyltransferase (EC 2.7.8.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phosphopentomutase (EC 5.4.2.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS system, N-acetylglucosamine-specific IIC component (EC 2.7.1.69)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphopantetheine adenylyltransferase (EC 2.7.7.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proline racemase (EC 5.1.1.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-hydroxy-3-methylbut-2-enyl diphosphate reductase (EC 1.17.1.2)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.3645</t>
@@ -75,40 +316,10 @@
     <t xml:space="preserve">uracil phosphoribosyltransferase (EC 2.4.2.9)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.3245</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTS system, N-acetylglucosamine-specific IIC component (EC 2.7.1.69)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.755</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formate--tetrahydrofolate ligase (EC 6.3.4.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substrate-specific component TrpP of tryptophan ECF transporter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP synthase epsilon chain (EC 3.6.3.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acetate kinase (EC 2.7.2.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3409</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valyl-tRNA synthetase (EC 6.1.1.9)</t>
+    <t xml:space="preserve">272563.8.peg.2711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phosphopantothenoylcysteine decarboxylase (EC 4.1.1.36)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.1284</t>
@@ -117,70 +328,46 @@
     <t xml:space="preserve">pyrimidine-nucleoside phosphorylase (EC 2.4.2.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.1061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-acetylgalactosamine-6-phosphate deacetylase | nagA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1382</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riboflavin kinase (EC 2.7.1.26)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphoenolpyruvate-protein phosphotransferase of PTS system (EC 2.7.3.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyruvate-flavodoxin oxidoreductase (EC 1.2.7.-)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isoleucyl-tRNA synthetase (EC 6.1.1.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trehalose-6-phosphate hydrolase (EC 3.2.1.93)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyrroline-5-carboxylate reductase (EC 1.5.1.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphoribosylamine--glycine ligase (EC 6.3.4.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cytidine deaminase (EC 3.5.4.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1406</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alanine transaminase (EC 2.6.1.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2644</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leucyl-tRNA synthetase (EC 6.1.1.4)</t>
+    <t xml:space="preserve">272563.8.peg.2551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glycyl-tRNA synthetase beta chain (EC 6.1.1.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS system, glucitol/sorbitol-specific IIC component (EC 2.7.1.69)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.3722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lysyl-tRNA synthetase (class II) (EC 6.1.1.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC transporter, ATP-binding protein (cluster 3, basic aa/glutamine/opines)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.2166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutaminyl-tRNA synthetase (EC 6.1.1.18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium:alanine symporter family protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyrosyl-tRNA synthetase (EC 6.1.1.1)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.128</t>
@@ -189,28 +376,22 @@
     <t xml:space="preserve">phosphate butyryltransferase (EC 2.3.1.19)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2469</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycine reductase component B beta subunit (EC 1.21.4.2) / Glycine reductase component B alpha subunit (EC 1.21.4.2) | grdE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3565</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UDP-N-acetylenolpyruvoylglucosamine reductase (EC 1.1.1.158)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1283</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purine nucleoside phosphorylase (EC 2.4.2.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphoribosylformylglycinamidine synthase, glutamine amidotransferase subunit (EC 6.3.5.3)</t>
+    <t xml:space="preserve">272563.8.peg.139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDP-N-acetylglucosamine 1-carboxyvinyltransferase (EC 2.5.1.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.1565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA-3-methyladenine glycosylase II (EC 3.2.2.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272563.8.peg.601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Threonyl-tRNA synthetase (EC 6.1.1.3)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.105</t>
@@ -219,34 +400,10 @@
     <t xml:space="preserve">Adenylate kinase (EC 2.7.4.3)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UDP-N-acetylmuramoylalanine--D-glutamate ligase (EC 6.3.2.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glucose-6-phosphate isomerase (EC 5.3.1.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1266</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-deoxy-D-xylulose 5-phosphate synthase (EC 2.2.1.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adenine phosphoribosyltransferase (EC 2.4.2.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1394</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDP-diacylglycerol--glycerol-3-phosphate 3-phosphatidyltransferase (EC 2.7.8.5)</t>
+    <t xml:space="preserve">272563.8.peg.1264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2E,6E)-farnesyl diphosphate synthase (EC 2.5.1.10)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.3557</t>
@@ -255,136 +412,16 @@
     <t xml:space="preserve">Pyruvate kinase (EC 2.7.1.40)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphopantetheine adenylyltransferase (EC 2.7.7.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sodium-solute symporter, putative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1908</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-hydroxy-3-methylbut-2-enyl diphosphate reductase (EC 1.17.1.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3634</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP synthase gamma chain (EC 3.6.3.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2711</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phosphopantothenoylcysteine decarboxylase (EC 4.1.1.36)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTS system, glucitol/sorbitol-specific IIB component (EC 2.7.1.198) / PTS system, glucitol/sorbitol-specific IIC component 2 | srlE_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2551</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycyl-tRNA synthetase beta chain (EC 6.1.1.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.202</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aspartate carbamoyltransferase (EC 2.1.3.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3722</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lysyl-tRNA synthetase (class II) (EC 6.1.1.6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-acetylneuraminate lyase (EC 4.1.3.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glutaminyl-tRNA synthetase (EC 6.1.1.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proline racemase (EC 5.1.1.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyrosyl-tRNA synthetase (EC 6.1.1.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.3635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP synthase alpha chain (EC 3.6.3.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UDP-N-acetylglucosamine 1-carboxyvinyltransferase (EC 2.5.1.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.766</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycine cleavage system H protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.601</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Threonyl-tRNA synthetase (EC 6.1.1.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1864</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC transporter, ATP-binding protein (cluster 3, basic aa/glutamine/opines)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.1264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2E,6E)-farnesyl diphosphate synthase (EC 2.5.1.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">272563.8.peg.2536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTS system, glucitol/sorbitol-specific IIC component (EC 2.7.1.69)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.735</t>
   </si>
   <si>
     <t xml:space="preserve">Phenylalanyl-tRNA synthetase beta chain (EC 6.1.1.20)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2754</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glycerol-3-phosphate dehydrogenase [NAD(P)+] (EC 1.1.1.94)</t>
+    <t xml:space="preserve">272563.120.peg.2623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspartate aminotransferase (EC 2.6.1.1)</t>
   </si>
   <si>
     <t xml:space="preserve">272563.8.peg.2552</t>
@@ -393,132 +430,66 @@
     <t xml:space="preserve">Glycyl-tRNA synthetase alpha chain (EC 6.1.1.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.3323</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triosephosphate isomerase (EC 5.3.1.1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.818</t>
   </si>
   <si>
     <t xml:space="preserve">Multimodular transpeptidase-transglycosylase (EC 2.4.1.129) (EC 3.4.-.-)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.1565</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA-3-methyladenine glycosylase II (EC 3.2.2.21)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.636</t>
   </si>
   <si>
     <t xml:space="preserve">Chloride channel protein</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.866</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glutamate synthase [NADPH] large chain (EC 1.4.1.13)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.1781</t>
   </si>
   <si>
     <t xml:space="preserve">Sulfur carrier protein ThiS subunit</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2720</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyrimidine operon regulatory protein PyrR</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2733</t>
   </si>
   <si>
     <t xml:space="preserve">Tryptophanyl-tRNA synthetase (EC 6.1.1.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.1282</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phosphopentomutase (EC 5.4.2.7)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2867</t>
   </si>
   <si>
     <t xml:space="preserve">Histidyl-tRNA synthetase (EC 6.1.1.21)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.3636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP synthase delta chain (EC 3.6.3.14)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2243</t>
   </si>
   <si>
     <t xml:space="preserve">1-deoxy-D-xylulose 5-phosphate reductoisomerase (EC 1.1.1.267)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.2488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-aspartate oxidase (EC 1.4.3.16)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2866</t>
   </si>
   <si>
     <t xml:space="preserve">Aspartyl-tRNA synthetase (EC 6.1.1.12)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.1574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyribose-phosphate aldolase (EC 4.1.2.4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2946</t>
   </si>
   <si>
     <t xml:space="preserve">dihydrofolate reductase (EC 1.5.1.3)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manganese-dependent inorganic pyrophosphatase (EC 3.6.1.1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.423</t>
   </si>
   <si>
     <t xml:space="preserve">Fructose-bisphosphate aldolase class II (EC 4.1.2.13)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.3633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP synthase beta chain (EC 3.6.3.14)</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.3718</t>
   </si>
   <si>
     <t xml:space="preserve">Thymidylate kinase (EC 2.7.4.9)</t>
   </si>
   <si>
-    <t xml:space="preserve">272563.8.peg.1774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodium:alanine symporter family protein</t>
-  </si>
-  <si>
     <t xml:space="preserve">272563.8.peg.2779</t>
   </si>
   <si>
@@ -750,181 +721,364 @@
     <t xml:space="preserve">amidophosphoribosyltransferase (EC 2.4.2.14)</t>
   </si>
   <si>
+    <t xml:space="preserve">Exchange reaction ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Substrate</t>
   </si>
   <si>
-    <t xml:space="preserve">Low_spores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High_spores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norm_low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norm_high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perc_diff</t>
+    <t xml:space="preserve">Median optimal flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00009_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00011_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00013_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ammonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00023_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Glutamate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00027_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Glucose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00029_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00030_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mn2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00035_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Alanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00039_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Lysine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00041_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Aspartate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00047_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00051_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Arginine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00054_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Serine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00060_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Methionine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00063_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ca2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00065_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Tryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00066_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Phenylalanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00067_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00069_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Tyrosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00084_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Cysteine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00099_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00104_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biotin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00107_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Leucine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00117_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Alanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00119_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Histidine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00122_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Acetyl-D-glucosamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00132_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Asparagine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00133_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicotinamide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00149_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00156_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Valine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00161_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Threonine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00186_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Glutamate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00205_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00207_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00220_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riboflavin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00226_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypoxanthine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00232_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Acetyl-Neuraminic acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00246_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00254_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00263_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyridoxol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00277_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxyguanosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00307_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00311_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guanosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00322_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L-Isoleucine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00393_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Folate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00412_e</t>
   </si>
   <si>
     <t xml:space="preserve">Deoxyuridine</t>
   </si>
   <si>
-    <t xml:space="preserve">Cl-</t>
+    <t xml:space="preserve">EX_cpd00438_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxyadenosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00567_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Proline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00644_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantothenate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00654_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deoxycytidine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00971_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd01711_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isobutyrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd05178_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isovalerate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd10515_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fe2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd19585_e</t>
   </si>
   <si>
     <t xml:space="preserve">2-Methylbutyrate</t>
   </si>
   <si>
-    <t xml:space="preserve">L-Cysteine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ca2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biotin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Tyrosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Phenylalanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Isoleucine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-Acetyl-Neuraminic acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Glutamate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantothenate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Threonine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicotinamide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Proline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guanosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Lysine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fe2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Serine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Co2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mn2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Tryptophan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Riboflavin</t>
+    <t xml:space="preserve">EX_cpd00001_e</t>
   </si>
   <si>
     <t xml:space="preserve">H2O</t>
   </si>
   <si>
-    <t xml:space="preserve">Cytosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Alanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Methionine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acetate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Leucine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Glutamate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-Cresol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D-Alanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Aspartate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyadenosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Arginine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Asparagine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxycytidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-Acetyl-D-glucosamine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Valine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pyridoxol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L-Histidine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isovalerate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deoxyguanosine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formate</t>
+    <t xml:space="preserve">EX_cpd00182_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adenosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00276_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Glucosamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_cpd00492_e</t>
   </si>
   <si>
     <t xml:space="preserve">N-Acetyl-D-mannosamine</t>
@@ -955,9 +1109,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -1082,8 +1235,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1105,8 +1258,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1121,7 +1274,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="55.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="2.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="54.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="54.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -1158,506 +1311,506 @@
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>26</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="E6" s="7" t="s">
         <v>38</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="E8" s="7" t="s">
         <v>50</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>56</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>60</v>
+      <c r="D10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>64</v>
+      <c r="D11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>68</v>
+      <c r="D12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>76</v>
+      <c r="D14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>80</v>
+      <c r="D15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>84</v>
+      <c r="D16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>88</v>
+      <c r="D17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>92</v>
+      <c r="D18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>96</v>
+      <c r="D19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>100</v>
+      <c r="D20" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>104</v>
+      <c r="D21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>108</v>
+      <c r="D22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>112</v>
+      <c r="D23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>120</v>
+      <c r="D25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>128</v>
-      </c>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
@@ -1667,421 +1820,391 @@
         <v>146</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>148</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C75" s="2"/>
     </row>
@@ -4876,1306 +4999,637 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>246</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>-221.6781</v>
+        <v>235</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>236</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>-175.0813</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <f aca="false">(B2/(B2+C2))*100</f>
-        <v>55.8721734129046</v>
-      </c>
-      <c r="E2" s="7" t="n">
-        <f aca="false">(C2/(B2+C2)*100)</f>
-        <v>44.1278265870954</v>
-      </c>
-      <c r="F2" s="7" t="n">
-        <f aca="false">ABS(D2-E2)</f>
-        <v>11.7443468258093</v>
+        <v>-43.6393702692397</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>-0.0617</v>
+        <v>237</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>238</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <f aca="false">(B3/(B3+C3))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <f aca="false">(C3/(B3+C3)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <f aca="false">ABS(D3-E3)</f>
-        <v>11.7753623188406</v>
+        <v>602.531976265822</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>677.5785</v>
+        <v>239</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>240</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>461.6247</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <f aca="false">(B4/(B4+C4))*100</f>
-        <v>59.478282715498</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <f aca="false">(C4/(B4+C4)*100)</f>
-        <v>40.521717284502</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <f aca="false">ABS(D4-E4)</f>
-        <v>18.956565430996</v>
+        <v>753.490177076425</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>-1.6588</v>
+        <v>241</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>242</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>-1.3101</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <f aca="false">(B5/(B5+C5))*100</f>
-        <v>55.8725453871804</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <f aca="false">(C5/(B5+C5)*100)</f>
-        <v>44.1274546128196</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <f aca="false">ABS(D5-E5)</f>
-        <v>11.7450907743609</v>
+        <v>-14.8504742212844</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>-0.0617</v>
+        <v>243</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>244</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <f aca="false">(B6/(B6+C6))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <f aca="false">(C6/(B6+C6)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <f aca="false">ABS(D6-E6)</f>
-        <v>11.7753623188406</v>
+        <v>-0.133410317696246</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>-0.0617</v>
+        <v>245</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>246</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <f aca="false">(B7/(B7+C7))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <f aca="false">(C7/(B7+C7)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <f aca="false">ABS(D7-E7)</f>
-        <v>11.7753623188406</v>
+        <v>729.570394923719</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>-222.3209</v>
+        <v>247</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>248</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>-59.6143</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <f aca="false">(B8/(B8+C8))*100</f>
-        <v>78.8553185270942</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <f aca="false">(C8/(B8+C8)*100)</f>
-        <v>21.1446814729058</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <f aca="false">ABS(D8-E8)</f>
-        <v>57.7106370541883</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>-0.0617</v>
+        <v>249</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>250</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <f aca="false">(B9/(B9+C9))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <f aca="false">(C9/(B9+C9)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <f aca="false">ABS(D9-E9)</f>
-        <v>11.7753623188406</v>
+        <v>-609.119072657253</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>-5.4018</v>
+        <v>251</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>252</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>-4.2663</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <f aca="false">(B10/(B10+C10))*100</f>
-        <v>55.8724051261365</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <f aca="false">(C10/(B10+C10)*100)</f>
-        <v>44.1275948738635</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <f aca="false">ABS(D10-E10)</f>
-        <v>11.7448102522729</v>
+        <v>-36.8060007907387</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>-690.5062</v>
+        <v>253</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>254</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>-471.7901</v>
-      </c>
-      <c r="D11" s="7" t="n">
-        <f aca="false">(B11/(B11+C11))*100</f>
-        <v>59.4087927493188</v>
-      </c>
-      <c r="E11" s="7" t="n">
-        <f aca="false">(C11/(B11+C11)*100)</f>
-        <v>40.5912072506813</v>
-      </c>
-      <c r="F11" s="7" t="n">
-        <f aca="false">ABS(D11-E11)</f>
-        <v>18.8175854986375</v>
+        <v>-33.383073210987</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>-550.9492</v>
+        <v>255</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>256</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>-59.4171</v>
-      </c>
-      <c r="D12" s="7" t="n">
-        <f aca="false">(B12/(B12+C12))*100</f>
-        <v>90.2653373883847</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <f aca="false">(C12/(B12+C12)*100)</f>
-        <v>9.73466261161535</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <f aca="false">ABS(D12-E12)</f>
-        <v>80.5306747767693</v>
+        <v>823.374803488087</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>82.3264</v>
+        <v>257</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>258</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>453.842</v>
-      </c>
-      <c r="D13" s="7" t="n">
-        <f aca="false">(B13/(B13+C13))*100</f>
-        <v>15.3545788972271</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <f aca="false">(C13/(B13+C13)*100)</f>
-        <v>84.6454211027729</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <f aca="false">ABS(D13-E13)</f>
-        <v>69.2908422055459</v>
+        <v>-4.87900590432321</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>-0.1295</v>
-      </c>
       <c r="C14" s="0" t="n">
-        <v>-0.1023</v>
-      </c>
-      <c r="D14" s="7" t="n">
-        <f aca="false">(B14/(B14+C14))*100</f>
-        <v>55.8671268334771</v>
-      </c>
-      <c r="E14" s="7" t="n">
-        <f aca="false">(C14/(B14+C14)*100)</f>
-        <v>44.1328731665229</v>
-      </c>
-      <c r="F14" s="7" t="n">
-        <f aca="false">ABS(D14-E14)</f>
-        <v>11.7342536669543</v>
+        <v>-287.934924010431</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>841.7361</v>
+      <c r="B15" s="0" t="s">
+        <v>262</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>662.2467</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <f aca="false">(B15/(B15+C15))*100</f>
-        <v>55.9671360603326</v>
-      </c>
-      <c r="E15" s="7" t="n">
-        <f aca="false">(C15/(B15+C15)*100)</f>
-        <v>44.0328639396674</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <f aca="false">ABS(D15-E15)</f>
-        <v>11.9342721206652</v>
+        <v>-4.11666123177281</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>-35.2989</v>
+        <v>263</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>264</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>-27.8791</v>
-      </c>
-      <c r="D16" s="7" t="n">
-        <f aca="false">(B16/(B16+C16))*100</f>
-        <v>55.8721390357403</v>
-      </c>
-      <c r="E16" s="7" t="n">
-        <f aca="false">(C16/(B16+C16)*100)</f>
-        <v>44.1278609642597</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <f aca="false">ABS(D16-E16)</f>
-        <v>11.7442780714806</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>-6.1171</v>
+        <v>265</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>266</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>-4.8313</v>
-      </c>
-      <c r="D17" s="7" t="n">
-        <f aca="false">(B17/(B17+C17))*100</f>
-        <v>55.8720908991268</v>
-      </c>
-      <c r="E17" s="7" t="n">
-        <f aca="false">(C17/(B17+C17)*100)</f>
-        <v>44.1279091008732</v>
-      </c>
-      <c r="F17" s="7" t="n">
-        <f aca="false">ABS(D17-E17)</f>
-        <v>11.7441817982536</v>
+        <v>-0.975801180864664</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>-0.3083</v>
+        <v>267</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>268</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>-0.2435</v>
-      </c>
-      <c r="D18" s="7" t="n">
-        <f aca="false">(B18/(B18+C18))*100</f>
-        <v>55.8716926422617</v>
-      </c>
-      <c r="E18" s="7" t="n">
-        <f aca="false">(C18/(B18+C18)*100)</f>
-        <v>44.1283073577383</v>
-      </c>
-      <c r="F18" s="7" t="n">
-        <f aca="false">ABS(D18-E18)</f>
-        <v>11.7433852845234</v>
+        <v>-6.67813933154247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>-99.3712</v>
+        <v>269</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>270</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>-465.7166</v>
-      </c>
-      <c r="D19" s="7" t="n">
-        <f aca="false">(B19/(B19+C19))*100</f>
-        <v>17.5850903169384</v>
-      </c>
-      <c r="E19" s="7" t="n">
-        <f aca="false">(C19/(B19+C19)*100)</f>
-        <v>82.4149096830616</v>
-      </c>
-      <c r="F19" s="7" t="n">
-        <f aca="false">ABS(D19-E19)</f>
-        <v>64.8298193661233</v>
+        <v>-719.31146401544</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>386.9759</v>
+        <v>271</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>272</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>334.8218</v>
-      </c>
-      <c r="D20" s="7" t="n">
-        <f aca="false">(B20/(B20+C20))*100</f>
-        <v>53.6127920607118</v>
-      </c>
-      <c r="E20" s="7" t="n">
-        <f aca="false">(C20/(B20+C20)*100)</f>
-        <v>46.3872079392882</v>
-      </c>
-      <c r="F20" s="7" t="n">
-        <f aca="false">ABS(D20-E20)</f>
-        <v>7.2255841214235</v>
+        <v>-6.34270767562032</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>-845.1678</v>
+        <v>273</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>274</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>-506.8009</v>
-      </c>
-      <c r="D21" s="7" t="n">
-        <f aca="false">(B21/(B21+C21))*100</f>
-        <v>62.5138584939134</v>
-      </c>
-      <c r="E21" s="7" t="n">
-        <f aca="false">(C21/(B21+C21)*100)</f>
-        <v>37.4861415060866</v>
-      </c>
-      <c r="F21" s="7" t="n">
-        <f aca="false">ABS(D21-E21)</f>
-        <v>25.0277169878267</v>
+        <v>-2.0507071691606</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>-29.7716</v>
+        <v>275</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>276</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>-23.5136</v>
-      </c>
-      <c r="D22" s="7" t="n">
-        <f aca="false">(B22/(B22+C22))*100</f>
-        <v>55.8721746376104</v>
-      </c>
-      <c r="E22" s="7" t="n">
-        <f aca="false">(C22/(B22+C22)*100)</f>
-        <v>44.1278253623896</v>
-      </c>
-      <c r="F22" s="7" t="n">
-        <f aca="false">ABS(D22-E22)</f>
-        <v>11.7443492752209</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>-0.0617</v>
+        <v>277</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>278</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D23" s="7" t="n">
-        <f aca="false">(B23/(B23+C23))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E23" s="7" t="n">
-        <f aca="false">(C23/(B23+C23)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F23" s="7" t="n">
-        <f aca="false">ABS(D23-E23)</f>
-        <v>11.7753623188406</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>-435.9503</v>
+        <v>279</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>280</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>-508.7071</v>
-      </c>
-      <c r="D24" s="7" t="n">
-        <f aca="false">(B24/(B24+C24))*100</f>
-        <v>46.1490377357971</v>
-      </c>
-      <c r="E24" s="7" t="n">
-        <f aca="false">(C24/(B24+C24)*100)</f>
-        <v>53.8509622642029</v>
-      </c>
-      <c r="F24" s="7" t="n">
-        <f aca="false">ABS(D24-E24)</f>
-        <v>7.70192452840574</v>
+        <v>-30.7194345297961</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>-0.0617</v>
+        <v>281</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>282</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D25" s="7" t="n">
-        <f aca="false">(B25/(B25+C25))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E25" s="7" t="n">
-        <f aca="false">(C25/(B25+C25)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F25" s="7" t="n">
-        <f aca="false">ABS(D25-E25)</f>
-        <v>11.7753623188406</v>
+        <v>-80.0461906178041</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>-0.0617</v>
+        <v>283</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>284</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D26" s="7" t="n">
-        <f aca="false">(B26/(B26+C26))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E26" s="7" t="n">
-        <f aca="false">(C26/(B26+C26)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F26" s="7" t="n">
-        <f aca="false">ABS(D26-E26)</f>
-        <v>11.7753623188406</v>
+        <v>-2.07357750933738</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>-0.7893</v>
+        <v>285</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>286</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>-0.6234</v>
-      </c>
-      <c r="D27" s="7" t="n">
-        <f aca="false">(B27/(B27+C27))*100</f>
-        <v>55.8717349755787</v>
-      </c>
-      <c r="E27" s="7" t="n">
-        <f aca="false">(C27/(B27+C27)*100)</f>
-        <v>44.1282650244213</v>
-      </c>
-      <c r="F27" s="7" t="n">
-        <f aca="false">ABS(D27-E27)</f>
-        <v>11.7434699511574</v>
+        <v>891.610781216804</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>-0.0678</v>
+        <v>287</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>288</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>-0.0536</v>
-      </c>
-      <c r="D28" s="7" t="n">
-        <f aca="false">(B28/(B28+C28))*100</f>
-        <v>55.8484349258649</v>
-      </c>
-      <c r="E28" s="7" t="n">
-        <f aca="false">(C28/(B28+C28)*100)</f>
-        <v>44.1515650741351</v>
-      </c>
-      <c r="F28" s="7" t="n">
-        <f aca="false">ABS(D28-E28)</f>
-        <v>11.6968698517298</v>
+        <v>-9.81899938245056</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>-217.9982</v>
+        <v>289</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>290</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>19.9943</v>
-      </c>
-      <c r="D29" s="7" t="n">
-        <f aca="false">(B29/(B29+C29))*100</f>
-        <v>110.097932414463</v>
-      </c>
-      <c r="E29" s="7" t="n">
-        <f aca="false">(C29/(B29+C29)*100)</f>
-        <v>-10.0979324144625</v>
-      </c>
-      <c r="F29" s="7" t="n">
-        <f aca="false">ABS(D29-E29)</f>
-        <v>120.195864828925</v>
+        <v>-0.381172336279917</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>210.3064</v>
+        <v>291</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>292</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>166.0999</v>
-      </c>
-      <c r="D30" s="7" t="n">
-        <f aca="false">(B30/(B30+C30))*100</f>
-        <v>55.8721785474898</v>
-      </c>
-      <c r="E30" s="7" t="n">
-        <f aca="false">(C30/(B30+C30)*100)</f>
-        <v>44.1278214525102</v>
-      </c>
-      <c r="F30" s="7" t="n">
-        <f aca="false">ABS(D30-E30)</f>
-        <v>11.7443570949795</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>-0.0617</v>
+        <v>293</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>294</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D31" s="7" t="n">
-        <f aca="false">(B31/(B31+C31))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E31" s="7" t="n">
-        <f aca="false">(C31/(B31+C31)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F31" s="7" t="n">
-        <f aca="false">ABS(D31-E31)</f>
-        <v>11.7753623188406</v>
+        <v>-29.2625395648944</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>-43.4487</v>
+        <v>295</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>296</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>-34.3158</v>
-      </c>
-      <c r="D32" s="7" t="n">
-        <f aca="false">(B32/(B32+C32))*100</f>
-        <v>55.8721524603129</v>
-      </c>
-      <c r="E32" s="7" t="n">
-        <f aca="false">(C32/(B32+C32)*100)</f>
-        <v>44.1278475396871</v>
-      </c>
-      <c r="F32" s="7" t="n">
-        <f aca="false">ABS(D32-E32)</f>
-        <v>11.7443049206257</v>
+        <v>-7.56245915170109</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>-3.3299</v>
+        <v>297</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>298</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>-2.6299</v>
-      </c>
-      <c r="D33" s="7" t="n">
-        <f aca="false">(B33/(B33+C33))*100</f>
-        <v>55.872680291285</v>
-      </c>
-      <c r="E33" s="7" t="n">
-        <f aca="false">(C33/(B33+C33)*100)</f>
-        <v>44.1273197087151</v>
-      </c>
-      <c r="F33" s="7" t="n">
-        <f aca="false">ABS(D33-E33)</f>
-        <v>11.7453605825699</v>
+        <v>-45.7406803530305</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1000</v>
+        <v>299</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>300</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>512.5522</v>
-      </c>
-      <c r="D34" s="7" t="n">
-        <f aca="false">(B34/(B34+C34))*100</f>
-        <v>66.1134207467352</v>
-      </c>
-      <c r="E34" s="7" t="n">
-        <f aca="false">(C34/(B34+C34)*100)</f>
-        <v>33.8865792532648</v>
-      </c>
-      <c r="F34" s="7" t="n">
-        <f aca="false">ABS(D34-E34)</f>
-        <v>32.2268414934704</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>281</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>-11.2229</v>
+        <v>301</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>302</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>-83.537</v>
-      </c>
-      <c r="D35" s="7" t="n">
-        <f aca="false">(B35/(B35+C35))*100</f>
-        <v>11.843511865251</v>
-      </c>
-      <c r="E35" s="7" t="n">
-        <f aca="false">(C35/(B35+C35)*100)</f>
-        <v>88.156488134749</v>
-      </c>
-      <c r="F35" s="7" t="n">
-        <f aca="false">ABS(D35-E35)</f>
-        <v>76.312976269498</v>
+        <v>526.17968864827</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>-36.9986</v>
+        <v>303</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>304</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>-29.2215</v>
-      </c>
-      <c r="D36" s="7" t="n">
-        <f aca="false">(B36/(B36+C36))*100</f>
-        <v>55.8721596614925</v>
-      </c>
-      <c r="E36" s="7" t="n">
-        <f aca="false">(C36/(B36+C36)*100)</f>
-        <v>44.1278403385075</v>
-      </c>
-      <c r="F36" s="7" t="n">
-        <f aca="false">ABS(D36-E36)</f>
-        <v>11.744319322985</v>
+        <v>-0.0838579139805234</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="B37" s="0" t="n">
-        <v>216.7918</v>
+        <v>305</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>306</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>54.8277</v>
-      </c>
-      <c r="D37" s="7" t="n">
-        <f aca="false">(B37/(B37+C37))*100</f>
-        <v>79.8145199442603</v>
-      </c>
-      <c r="E37" s="7" t="n">
-        <f aca="false">(C37/(B37+C37)*100)</f>
-        <v>20.1854800557397</v>
-      </c>
-      <c r="F37" s="7" t="n">
-        <f aca="false">ABS(D37-E37)</f>
-        <v>59.6290398885205</v>
+        <v>305.482060672041</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>-0.0617</v>
+        <v>307</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>308</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D38" s="7" t="n">
-        <f aca="false">(B38/(B38+C38))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E38" s="7" t="n">
-        <f aca="false">(C38/(B38+C38)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F38" s="7" t="n">
-        <f aca="false">ABS(D38-E38)</f>
-        <v>11.7753623188406</v>
+        <v>-249.263487267384</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>-64.7476</v>
+        <v>309</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>310</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>-51.1376</v>
-      </c>
-      <c r="D39" s="7" t="n">
-        <f aca="false">(B39/(B39+C39))*100</f>
-        <v>55.8721907542982</v>
-      </c>
-      <c r="E39" s="7" t="n">
-        <f aca="false">(C39/(B39+C39)*100)</f>
-        <v>44.1278092457018</v>
-      </c>
-      <c r="F39" s="7" t="n">
-        <f aca="false">ABS(D39-E39)</f>
-        <v>11.7443815085964</v>
+        <v>-305.482060672042</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>-27.0028</v>
+        <v>311</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>312</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>-21.3268</v>
-      </c>
-      <c r="D40" s="7" t="n">
-        <f aca="false">(B40/(B40+C40))*100</f>
-        <v>55.8721777130372</v>
-      </c>
-      <c r="E40" s="7" t="n">
-        <f aca="false">(C40/(B40+C40)*100)</f>
-        <v>44.1278222869629</v>
-      </c>
-      <c r="F40" s="7" t="n">
-        <f aca="false">ABS(D40-E40)</f>
-        <v>11.7443554260743</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>7.4419</v>
+        <v>313</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>314</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>5.8776</v>
-      </c>
-      <c r="D41" s="7" t="n">
-        <f aca="false">(B41/(B41+C41))*100</f>
-        <v>55.872217425579</v>
-      </c>
-      <c r="E41" s="7" t="n">
-        <f aca="false">(C41/(B41+C41)*100)</f>
-        <v>44.127782574421</v>
-      </c>
-      <c r="F41" s="7" t="n">
-        <f aca="false">ABS(D41-E41)</f>
-        <v>11.7444348511581</v>
+        <v>-0.0762344672551762</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>814.15</v>
+        <v>315</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>316</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>135.7354</v>
-      </c>
-      <c r="D42" s="7" t="n">
-        <f aca="false">(B42/(B42+C42))*100</f>
-        <v>85.7103393735708</v>
-      </c>
-      <c r="E42" s="7" t="n">
-        <f aca="false">(C42/(B42+C42)*100)</f>
-        <v>14.2896606264293</v>
-      </c>
-      <c r="F42" s="7" t="n">
-        <f aca="false">ABS(D42-E42)</f>
-        <v>71.4206787471415</v>
+        <v>-133.440740949972</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="B43" s="0" t="n">
-        <v>-3.9465</v>
+        <v>317</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>318</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>-3.117</v>
-      </c>
-      <c r="D43" s="7" t="n">
-        <f aca="false">(B43/(B43+C43))*100</f>
-        <v>55.8717349755787</v>
-      </c>
-      <c r="E43" s="7" t="n">
-        <f aca="false">(C43/(B43+C43)*100)</f>
-        <v>44.1282650244213</v>
-      </c>
-      <c r="F43" s="7" t="n">
-        <f aca="false">ABS(D43-E43)</f>
-        <v>11.7434699511574</v>
+        <v>259.997650573351</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>-7.9424</v>
+        <v>319</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>320</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>-6.2729</v>
-      </c>
-      <c r="D44" s="7" t="n">
-        <f aca="false">(B44/(B44+C44))*100</f>
-        <v>55.8721940444451</v>
-      </c>
-      <c r="E44" s="7" t="n">
-        <f aca="false">(C44/(B44+C44)*100)</f>
-        <v>44.1278059555549</v>
-      </c>
-      <c r="F44" s="7" t="n">
-        <f aca="false">ABS(D44-E44)</f>
-        <v>11.7443880888901</v>
+        <v>-324.1843337236</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>-1.9424</v>
+        <v>321</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>322</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>-1.5341</v>
-      </c>
-      <c r="D45" s="7" t="n">
-        <f aca="false">(B45/(B45+C45))*100</f>
-        <v>55.8722853444556</v>
-      </c>
-      <c r="E45" s="7" t="n">
-        <f aca="false">(C45/(B45+C45)*100)</f>
-        <v>44.1277146555444</v>
-      </c>
-      <c r="F45" s="7" t="n">
-        <f aca="false">ABS(D45-E45)</f>
-        <v>11.7445706889113</v>
+        <v>-788.507959309513</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>-0.0617</v>
+        <v>323</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>324</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D46" s="7" t="n">
-        <f aca="false">(B46/(B46+C46))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E46" s="7" t="n">
-        <f aca="false">(C46/(B46+C46)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F46" s="7" t="n">
-        <f aca="false">ABS(D46-E46)</f>
-        <v>11.7753623188406</v>
+        <v>-0.0762344672550626</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>-174.5069</v>
+        <v>325</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>326</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>-325.8059</v>
-      </c>
-      <c r="D47" s="7" t="n">
-        <f aca="false">(B47/(B47+C47))*100</f>
-        <v>34.8795593476721</v>
-      </c>
-      <c r="E47" s="7" t="n">
-        <f aca="false">(C47/(B47+C47)*100)</f>
-        <v>65.1204406523279</v>
-      </c>
-      <c r="F47" s="7" t="n">
-        <f aca="false">ABS(D47-E47)</f>
-        <v>30.2408813046558</v>
+        <v>-274.056211821616</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>787.6285</v>
+        <v>327</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>328</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>498.7811</v>
-      </c>
-      <c r="D48" s="7" t="n">
-        <f aca="false">(B48/(B48+C48))*100</f>
-        <v>61.2268829461472</v>
-      </c>
-      <c r="E48" s="7" t="n">
-        <f aca="false">(C48/(B48+C48)*100)</f>
-        <v>38.7731170538528</v>
-      </c>
-      <c r="F48" s="7" t="n">
-        <f aca="false">ABS(D48-E48)</f>
-        <v>22.4537658922943</v>
+        <v>9.20031246469273</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>-8.0904</v>
+        <v>329</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>330</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>-6.3898</v>
-      </c>
-      <c r="D49" s="7" t="n">
-        <f aca="false">(B49/(B49+C49))*100</f>
-        <v>55.8721564619273</v>
-      </c>
-      <c r="E49" s="7" t="n">
-        <f aca="false">(C49/(B49+C49)*100)</f>
-        <v>44.1278435380727</v>
-      </c>
-      <c r="F49" s="7" t="n">
-        <f aca="false">ABS(D49-E49)</f>
-        <v>11.7443129238546</v>
+        <v>-4.17764880557684</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>-0.0617</v>
+        <v>331</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>332</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>-0.0487</v>
-      </c>
-      <c r="D50" s="7" t="n">
-        <f aca="false">(B50/(B50+C50))*100</f>
-        <v>55.8876811594203</v>
-      </c>
-      <c r="E50" s="7" t="n">
-        <f aca="false">(C50/(B50+C50)*100)</f>
-        <v>44.1123188405797</v>
-      </c>
-      <c r="F50" s="7" t="n">
-        <f aca="false">ABS(D50-E50)</f>
-        <v>11.7753623188406</v>
+        <v>-0.160092381235359</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>-1.6773</v>
+        <v>333</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>334</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>-1.3247</v>
-      </c>
-      <c r="D51" s="7" t="n">
-        <f aca="false">(B51/(B51+C51))*100</f>
-        <v>55.8727514990007</v>
-      </c>
-      <c r="E51" s="7" t="n">
-        <f aca="false">(C51/(B51+C51)*100)</f>
-        <v>44.1272485009993</v>
-      </c>
-      <c r="F51" s="7" t="n">
-        <f aca="false">ABS(D51-E51)</f>
-        <v>11.7455029980013</v>
+        <v>-2.40138571853407</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>0</v>
+        <v>335</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>336</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>74.6731</v>
-      </c>
-      <c r="D52" s="7" t="n">
-        <f aca="false">(B52/(B52+C52))*100</f>
-        <v>0</v>
-      </c>
-      <c r="E52" s="7" t="n">
-        <f aca="false">(C52/(B52+C52)*100)</f>
-        <v>100</v>
-      </c>
-      <c r="F52" s="7" t="n">
-        <f aca="false">ABS(D52-E52)</f>
-        <v>100</v>
+        <v>-0.0762344672546473</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>0</v>
+        <v>337</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>338</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>-2.9183</v>
-      </c>
-      <c r="D53" s="7" t="n">
-        <f aca="false">(B53/(B53+C53))*100</f>
-        <v>-0</v>
-      </c>
-      <c r="E53" s="7" t="n">
-        <f aca="false">(C53/(B53+C53)*100)</f>
-        <v>100</v>
-      </c>
-      <c r="F53" s="7" t="n">
-        <f aca="false">ABS(D53-E53)</f>
-        <v>100</v>
+        <v>16.7527800637106</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>263.7019</v>
+        <v>339</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>340</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" s="7" t="n">
-        <f aca="false">(B54/(B54+C54))*100</f>
-        <v>100</v>
-      </c>
-      <c r="E54" s="7" t="n">
-        <f aca="false">(C54/(B54+C54)*100)</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="7" t="n">
-        <f aca="false">ABS(D54-E54)</f>
-        <v>100</v>
+        <v>16.9348397411909</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>171.865</v>
+        <v>341</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>342</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="7" t="n">
-        <f aca="false">(B55/(B55+C55))*100</f>
-        <v>100</v>
-      </c>
-      <c r="E55" s="7" t="n">
-        <f aca="false">(C55/(B55+C55)*100)</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="7" t="n">
-        <f aca="false">ABS(D55-E55)</f>
-        <v>100</v>
+        <v>-0.0762344672551762</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>774.035769494173</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F30:F55 F2:F28">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF2A6099"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFC9211E"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F29">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF2A6099"/>
-        <color rgb="FFFFFFFF"/>
-        <color rgb="FFC9211E"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6191,62 +5645,686 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>-282.911466766835</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>-37.5978740658849</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>874.172642439786</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>810.65012843563</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>-12.7945535452464</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>999.999999999971</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>-0.0656804596777647</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>-559.191589576089</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>-31.7105259324707</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>-28.7614732929382</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>727.619146869368</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>-4.20354941938297</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>-118.370176846268</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>-3.54674482260441</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>-0.0656804596777647</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>-0.840709883876571</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>-5.75360826778041</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>-748.157586812738</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>-5.46461424519782</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>-1.76680436533451</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>-0.0656804596777647</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>-0.0656804596779352</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>-11.9538436613704</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>-68.9644826617529</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>-1.78650850323777</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>650.081267354436</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>-8.45964320650825</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>-0.328402298388426</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>-0.0656804596777647</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>-8.61727630973519</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>-6.51550160004365</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>348</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>-236.573105963226</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>-39.4082758067159</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>-0.0656804596779352</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>467.833530282334</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>-0.0722485056455753</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>-601.507739483399</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>-0.0656804596777647</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>-0.0656804596779352</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>38.5536421692844</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>224.003207731339</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>-471.207359508568</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>-907.678836831944</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>-0.0656804596778784</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>-236.115481856718</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>244.515983270739</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>10.9061343072077</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>-3.59928919034667</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>-0.137928965323397</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>-2.06893447985249</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>-0.0656804596770826</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>-0.0656804596779352</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>894.184992948797</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>303</v>
+        <v>354</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>305</v>
+        <v>356</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>306</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>307</v>
+        <v>358</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.75</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.149</v>
+        <v>0.162</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0.009</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.64</v>
+        <v>0.75</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.149</v>
+        <v>0.175</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0.0006</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>